<commit_message>
Update test results data - 2025-16-11 10:51 AM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 2.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\FBS Result Giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF68D189-8AF4-4BE8-9088-47C62B7281BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF8A577-224D-4501-8C31-97487BB2C655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1225,7 +1225,7 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="Y2">
         <f t="shared" ref="Y2:Y25" si="12">_xlfn.RANK.EQ(X2, $X$2:$X$1002, 0)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="19">
         <v>6</v>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF25" si="14">_xlfn.RANK.EQ(AE2, $AE$2:$AE$1002, 0)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AG2" s="13"/>
       <c r="AH2">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="Y3">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z3" s="20">
         <v>7</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="AF3">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AG3" s="13"/>
       <c r="AH3">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="Y4">
         <f t="shared" si="12"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z4" s="20">
         <v>5.5</v>
@@ -1672,7 +1672,7 @@
       </c>
       <c r="AF4">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AG4" s="13"/>
       <c r="AH4">
@@ -2031,7 +2031,7 @@
       </c>
       <c r="Y8">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z8" s="19">
         <v>5.5</v>
@@ -2052,7 +2052,7 @@
       </c>
       <c r="AF8">
         <f t="shared" si="14"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AI8">
         <v>-0.25</v>
@@ -2145,7 +2145,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Z9" s="19">
         <v>5</v>
@@ -2166,7 +2166,7 @@
       </c>
       <c r="AF9">
         <f t="shared" si="14"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2329,7 +2329,7 @@
       </c>
       <c r="Y11">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Z11" s="20">
         <v>6</v>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="AF11">
         <f t="shared" si="14"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2551,7 +2551,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Z13" s="19">
         <v>6</v>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="AF13">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="AF19">
         <f t="shared" si="14"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="Y21">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z21" s="19">
         <v>6.5</v>
@@ -3270,7 +3270,7 @@
       </c>
       <c r="AF21">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3281,46 +3281,46 @@
         <v>74</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
         <f t="shared" si="0"/>
-        <v>7.75</v>
+        <v>14.75</v>
       </c>
       <c r="F22">
         <f t="shared" si="1"/>
-        <v>48.4375</v>
+        <v>92.1875</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I22">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="J22">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>79.166666666666657</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M22">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N22">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -3337,30 +3337,30 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U22">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="V22">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>46.875</v>
       </c>
       <c r="W22">
         <f t="shared" si="10"/>
-        <v>7.75</v>
+        <v>37.75</v>
       </c>
       <c r="X22">
         <f t="shared" si="11"/>
-        <v>12.916666666666668</v>
+        <v>62.916666666666664</v>
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Z22" s="20">
         <v>7</v>
@@ -3377,11 +3377,11 @@
       </c>
       <c r="AE22">
         <f t="shared" si="13"/>
-        <v>32.25</v>
+        <v>62.25</v>
       </c>
       <c r="AF22">
         <f t="shared" si="14"/>
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
Update test results data - 2025-16-11 10:57 AM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 2.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF8A577-224D-4501-8C31-97487BB2C655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72FD28E-7743-4DCE-BC94-ECADDBE308A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
@@ -4781,11 +4781,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:BZ25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="BM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="CD16" sqref="CD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7441,41 +7441,111 @@
       <c r="K22" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="18"/>
-      <c r="V22" s="18"/>
-      <c r="W22" s="18"/>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="18"/>
-      <c r="Z22" s="18"/>
-      <c r="AA22" s="18"/>
-      <c r="AB22" s="18"/>
-      <c r="AC22" s="18"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="18"/>
-      <c r="AG22" s="18"/>
-      <c r="AH22" s="18"/>
-      <c r="AI22" s="18"/>
-      <c r="AJ22" s="18"/>
-      <c r="AK22" s="18"/>
-      <c r="AL22" s="18"/>
-      <c r="AM22" s="18"/>
-      <c r="AN22" s="18"/>
-      <c r="AO22" s="18"/>
-      <c r="AP22" s="18"/>
-      <c r="AQ22" s="18"/>
-      <c r="AR22" s="18"/>
-      <c r="AS22" s="18"/>
-      <c r="AT22" s="18"/>
+      <c r="L22" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="O22" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="P22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q22" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="R22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="S22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="T22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="U22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="V22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="W22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="X22" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AI22" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AK22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AM22" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AO22" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="AP22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AQ22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AR22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AS22" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="AT22" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="AU22" s="18"/>
       <c r="AV22" s="18"/>
       <c r="AW22" s="18"/>
@@ -7492,22 +7562,52 @@
       <c r="BH22" s="18"/>
       <c r="BI22" s="18"/>
       <c r="BJ22" s="18"/>
-      <c r="BK22" s="18"/>
-      <c r="BL22" s="18"/>
-      <c r="BM22" s="18"/>
-      <c r="BN22" s="18"/>
-      <c r="BO22" s="18"/>
-      <c r="BP22" s="18"/>
-      <c r="BQ22" s="18"/>
-      <c r="BR22" s="18"/>
-      <c r="BS22" s="18"/>
-      <c r="BT22" s="18"/>
-      <c r="BU22" s="18"/>
+      <c r="BK22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="BL22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="BM22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="BO22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="BP22" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="BQ22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="BR22" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BS22" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="BT22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="BU22" s="16" t="s">
+        <v>176</v>
+      </c>
       <c r="BV22" s="18"/>
-      <c r="BW22" s="18"/>
-      <c r="BX22" s="18"/>
-      <c r="BY22" s="18"/>
-      <c r="BZ22" s="18"/>
+      <c r="BW22" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="BX22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY22" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="BZ22" s="16" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="23" spans="1:78">
       <c r="A23" s="15" t="s">

</xml_diff>